<commit_message>
final revision for project upload
</commit_message>
<xml_diff>
--- a/0. Business Plan (Bus Entrep)/12monthcashflowFINAL.xlsx
+++ b/0. Business Plan (Bus Entrep)/12monthcashflowFINAL.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cedric\Desktop\AAA-ProjectDocs\AudioAcousticAssistan-AAA\0. Business Plan (Bus Entrep)\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
   </bookViews>
   <sheets>
     <sheet name="Twelve-month cash flow" sheetId="1" r:id="rId1"/>
@@ -189,9 +189,6 @@
     <t>Taxes</t>
   </si>
   <si>
-    <t>Audiotronics</t>
-  </si>
-  <si>
     <t>Capital purchase (Computers)</t>
   </si>
   <si>
@@ -199,6 +196,9 @@
   </si>
   <si>
     <t>Capital purchase (website)</t>
+  </si>
+  <si>
+    <t>AudioAcousticAssistant</t>
   </si>
 </sst>
 </file>
@@ -847,9 +847,9 @@
   </sheetPr>
   <dimension ref="B1:Q52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P47" sqref="P47"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -868,7 +868,7 @@
         <v>39</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I2" s="21"/>
       <c r="J2" s="21"/>
@@ -2165,7 +2165,7 @@
     </row>
     <row r="36" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C36" s="10">
         <v>5000</v>
@@ -2189,7 +2189,7 @@
     </row>
     <row r="37" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C37" s="10">
         <v>25</v>
@@ -2213,7 +2213,7 @@
     </row>
     <row r="38" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C38" s="10">
         <v>700</v>

</xml_diff>